<commit_message>
added minPA variation to mass_simulate
</commit_message>
<xml_diff>
--- a/beatthestreak/times/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/times/2010,2009,20,20,D Times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="0" windowWidth="23460" windowHeight="15380" tabRatio="500" firstSheet="17" activeTab="19"/>
+    <workbookView xWindow="840" yWindow="0" windowWidth="23460" windowHeight="15380" tabRatio="500" firstSheet="20" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,8 @@
     <sheet name="boxscoreBuffer installed" sheetId="18" r:id="rId18"/>
     <sheet name="extended batAveCSV" sheetId="19" r:id="rId19"/>
     <sheet name="optimized get_part_supserset" sheetId="20" r:id="rId20"/>
+    <sheet name="Installed player hit_info hash" sheetId="21" r:id="rId21"/>
+    <sheet name="removed update_bot_copy" sheetId="22" r:id="rId22"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="32">
   <si>
     <t>T1</t>
   </si>
@@ -117,6 +119,24 @@
   <si>
     <t>recalculate those values.</t>
   </si>
+  <si>
+    <t>Installed hash table-based lookup of player hit Infos (hitVals and otherInfo)</t>
+  </si>
+  <si>
+    <t>During setup, csv's of the player's hit info for the entire season</t>
+  </si>
+  <si>
+    <t>are generated, and then lazily loaded into a hash table</t>
+  </si>
+  <si>
+    <t>during the simulation</t>
+  </si>
+  <si>
+    <t>Update_bot_copy was actually slowing the sim down,</t>
+  </si>
+  <si>
+    <t>so I got rid of it</t>
+  </si>
 </sst>
 </file>
 
@@ -187,7 +207,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -245,8 +265,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -254,8 +276,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -284,6 +309,7 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -312,6 +338,7 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2409,8 +2436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2552,6 +2579,328 @@
         <f t="shared" si="1"/>
         <v>3.666666666666929E-3</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1.19</v>
+      </c>
+      <c r="C2">
+        <v>1.222</v>
+      </c>
+      <c r="D2">
+        <v>1.2</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>1.204</v>
+      </c>
+      <c r="F2" s="3">
+        <f>('optimized get_part_supserset'!E2-'Installed player hit_info hash'!E2)/'optimized get_part_supserset'!E2</f>
+        <v>0.35546038543897224</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41814</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1.105</v>
+      </c>
+      <c r="C3">
+        <v>1.1319999999999999</v>
+      </c>
+      <c r="D3">
+        <v>1.113</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>1.1166666666666667</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="C4">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>1.1859999999999999</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>1.2169999999999999</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1.196</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1996666666666667</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>5.0000000000001155E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>4.3333333333333002E-3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="7"/>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1.2509999999999999</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1.1359999999999999</v>
+      </c>
+      <c r="E2" s="9">
+        <f>AVERAGE(B2:D2)</f>
+        <v>1.1756666666666666</v>
+      </c>
+      <c r="F2" s="9">
+        <f>('Installed player hit_info hash'!E2-'removed update_bot_copy'!E2)/'Installed player hit_info hash'!E2</f>
+        <v>2.3532668881506083E-2</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41814</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1.0580000000000001</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1.1439999999999999</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1.0529999999999999</v>
+      </c>
+      <c r="E3" s="9">
+        <f t="shared" ref="E3:E6" si="0">AVERAGE(B3:D3)</f>
+        <v>1.085</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="7">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>7.8E-2</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="0"/>
+        <v>8.433333333333333E-2</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1.863</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1.861</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1.869</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.8643333333333334</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="7">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C6" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D6" s="7">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="0"/>
+        <v>3.6666666666666666E-3</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>